<commit_message>
Add .DS_Store files and update DiccPacientes.xlsx in Laboratorios
</commit_message>
<xml_diff>
--- a/Laboratorios/L1 Regresion Lineal/data/DiccPacientes.xlsx
+++ b/Laboratorios/L1 Regresion Lineal/data/DiccPacientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria Del Pilar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/s_gonzalezd_uniandes_edu_co/Documents/UNIV/2026-1/aprendizaje_maquina/aprendizaje-maquina/Laboratorios/L1 Regresion Lineal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{C17728EB-1387-446F-A2D5-23F312D41095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C361F363-4B6E-4C9B-BC2D-C48F2ADC5448}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29040" windowHeight="15720" xr2:uid="{C361F363-4B6E-4C9B-BC2D-C48F2ADC5448}"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario Pacientes-L1" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,18 +601,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61681A59-2BE2-45E6-973A-AD303FB886A6}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -634,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -645,7 +645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -656,7 +656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -667,7 +667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -678,7 +678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -689,7 +689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -700,7 +700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -711,7 +711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.5">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -722,7 +722,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -733,7 +733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="29.25">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -744,7 +744,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -755,7 +755,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29.25">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -766,7 +766,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29.25">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -777,7 +777,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -788,7 +788,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="43.5">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -799,7 +799,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -810,7 +810,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="29.25">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -821,7 +821,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -832,7 +832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -843,7 +843,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="43.5">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -854,7 +854,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29.25">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -865,7 +865,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -876,7 +876,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="29.25">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>55</v>
       </c>

</xml_diff>